<commit_message>
'ModBus Devices' - First Running '120_Storage' Version
</commit_message>
<xml_diff>
--- a/IPS Modebus Devices/Modbus Doku/Gen24_Primo_Symo_Inverter_Register_Map_Float_storage_ROW.xlsx
+++ b/IPS Modebus Devices/Modbus Doku/Gen24_Primo_Symo_Inverter_Register_Map_Float_storage_ROW.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProgramData\Symcon\modules\IPS_PG-Fronius\IPS Modebus Devices\Modbus Doku\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D29DCDF9-C685-4A00-A1E2-3E089838DFD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A160A8-6E65-4BEB-B665-DC41B2CEE935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36960" yWindow="450" windowWidth="20190" windowHeight="20880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5445" yWindow="1320" windowWidth="21795" windowHeight="19785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Complete Map" sheetId="1" r:id="rId1"/>
@@ -2151,8 +2151,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L248"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A231" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H221" sqref="H221"/>
+    <sheetView tabSelected="1" topLeftCell="A232" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K221" sqref="K221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>